<commit_message>
assignment 2: computational exploration
</commit_message>
<xml_diff>
--- a/UnitTests/FE640_set1_20.xlsx
+++ b/UnitTests/FE640_set1_20.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todd\Documents\forestry\OSU\FE 640\UnitTests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D61DA6-4DC4-4730-BACD-9D76EB456AAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAEF17A-C962-45D7-99CB-5DE0E8E05A0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3825" yWindow="570" windowWidth="20055" windowHeight="12075" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1260" yWindow="705" windowWidth="20055" windowHeight="12075" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="units" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>1st Period Volume</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>iterations</t>
+  </si>
+  <si>
+    <t>M iterations/s</t>
   </si>
 </sst>
 </file>
@@ -347,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -442,6 +445,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -48817,10 +48821,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -49083,145 +49087,158 @@
         <v>3000100</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="35" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="30">
+        <f>0.000001*B17/B16</f>
+        <v>7.0382953265765753</v>
+      </c>
+      <c r="C18" s="30">
+        <f>0.000001*C17/C16</f>
+        <v>11.905158730158728</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="37"/>
-      <c r="C19" s="36"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="9" t="s">
+      <c r="B20" s="37"/>
+      <c r="C20" s="36"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B21" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C21" s="16" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="18">
-        <v>440500</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="19">
-        <v>10000</v>
+        <v>37</v>
+      </c>
+      <c r="C22" s="18">
+        <v>440500</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B23" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="21">
-        <v>100</v>
+        <v>34</v>
+      </c>
+      <c r="C23" s="19">
+        <v>10000</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="21">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="21">
+      <c r="C25" s="21">
         <v>0.99995400000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="22" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B26" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="23">
+      <c r="C26" s="23">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="35" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="37"/>
-      <c r="C26" s="36"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
+      <c r="B27" s="37"/>
+      <c r="C27" s="36"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="9" t="s">
+      <c r="B28" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="16" t="s">
+      <c r="C28" s="16" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" s="18">
-        <v>440500</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="18">
+        <v>440500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B30" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C29" s="20" t="s">
+      <c r="C30" s="20" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="22" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B31" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="26">
+      <c r="C31" s="26">
         <v>10000</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="25"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-    </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="24"/>
-      <c r="B32" s="24"/>
-      <c r="C32" s="24"/>
+      <c r="A32" s="25"/>
+      <c r="B32" s="25"/>
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B1:C1"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A27:C27"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -71354,8 +71371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80FE5748-84A2-4EC6-A545-A97A691A5C01}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B101"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -71457,12 +71474,12 @@
         <v>44</v>
       </c>
       <c r="F5" s="30">
-        <f>_xlfn.STDEV.S(B2:B101)/1000000</f>
-        <v>1.1875041803865687E-2</v>
+        <f>_xlfn.STDEV.S(B2:B101)/1000</f>
+        <v>11.875041803865686</v>
       </c>
       <c r="G5" s="30">
-        <f>_xlfn.STDEV.S(C2:C101)/1000000</f>
-        <v>0.23379027997530999</v>
+        <f>_xlfn.STDEV.S(C2:C101)/1000</f>
+        <v>233.79027997531</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>